<commit_message>
Addition of heuristic decomp solution
</commit_message>
<xml_diff>
--- a/src/data/test_problems/4_comp_linear_hydrocarbons.xlsx
+++ b/src/data/test_problems/4_comp_linear_hydrocarbons.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Desktop\sns_modeling\src\data\poster_problem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Desktop\sns_modeling\src\data\test_problems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D394AC19-9C35-4CB4-A28F-2AFCE21CAD48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83036053-0D36-4A2F-9E5A-BE5CD034E2E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -461,7 +461,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -492,7 +492,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -501,12 +501,11 @@
         <v>85</v>
       </c>
       <c r="D2" s="1">
-        <f>1500/1000000</f>
-        <v>1.5E-3</v>
+        <f>150000/1000000</f>
+        <v>0.15</v>
       </c>
       <c r="E2" s="1">
-        <f>5000/1000000</f>
-        <v>5.0000000000000001E-3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -520,7 +519,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -571,7 +570,7 @@
         <v>0.1</v>
       </c>
       <c r="D2" s="2">
-        <v>8.9</v>
+        <v>12.1</v>
       </c>
       <c r="E2" s="2">
         <v>877</v>
@@ -623,7 +622,7 @@
         <v>0.4</v>
       </c>
       <c r="D4" s="2">
-        <v>3.2</v>
+        <v>3.8</v>
       </c>
       <c r="E4" s="2">
         <v>868</v>
@@ -649,7 +648,7 @@
         <v>0.25</v>
       </c>
       <c r="D5" s="2">
-        <v>1.55</v>
+        <v>1</v>
       </c>
       <c r="E5" s="2">
         <v>883</v>

</xml_diff>